<commit_message>
function composition standing implemented
</commit_message>
<xml_diff>
--- a/data/out/tb_wc_fifa.xlsx
+++ b/data/out/tb_wc_fifa.xlsx
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -502,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -526,13 +526,13 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -553,7 +553,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -562,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -589,10 +589,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -622,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -643,7 +643,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
@@ -652,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -676,13 +676,13 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -709,10 +709,10 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -742,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -763,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -796,13 +796,13 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -829,10 +829,10 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -862,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -883,7 +883,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -892,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -916,13 +916,13 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" t="n">
         <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -949,10 +949,10 @@
         <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -982,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1003,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1012,7 +1012,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1036,13 +1036,13 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1069,10 +1069,10 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1096,13 +1096,13 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -1120,7 +1120,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -1132,7 +1132,7 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -1153,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>1</v>
@@ -1162,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -1192,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
@@ -1210,7 +1210,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
         <v>1</v>
@@ -1222,7 +1222,7 @@
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -1246,13 +1246,13 @@
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -1279,10 +1279,10 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" t="n">
         <v>1</v>
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -1333,7 +1333,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>1</v>
@@ -1342,7 +1342,7 @@
         <v>1</v>
       </c>
       <c r="H30" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -1366,13 +1366,13 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -1399,10 +1399,10 @@
         <v>1</v>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
@@ -1420,7 +1420,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -1432,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1456,13 +1456,13 @@
         <v>1</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
         <v>1</v>
       </c>
       <c r="H34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -1483,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>1</v>
@@ -1492,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -1519,10 +1519,10 @@
         <v>1</v>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -1540,7 +1540,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1552,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1576,13 +1576,13 @@
         <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1603,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>1</v>
@@ -1612,7 +1612,7 @@
         <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -1639,10 +1639,10 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -1663,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -1672,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" t="n">
         <v>2</v>
@@ -1702,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
@@ -1726,13 +1726,13 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -1759,10 +1759,10 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
@@ -1780,13 +1780,13 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E45" t="n">
         <v>1</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
@@ -1813,7 +1813,7 @@
         <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1822,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
@@ -1849,10 +1849,10 @@
         <v>1</v>
       </c>
       <c r="G47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -1873,10 +1873,10 @@
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G48" t="n">
         <v>1</v>
@@ -1906,13 +1906,13 @@
         <v>1</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" t="n">
         <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -1930,7 +1930,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
         <v>1</v>
@@ -1942,7 +1942,7 @@
         <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -1969,10 +1969,10 @@
         <v>1</v>
       </c>
       <c r="G51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52">
@@ -1993,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>1</v>
@@ -2002,7 +2002,7 @@
         <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
@@ -2020,7 +2020,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E53" t="n">
         <v>1</v>
@@ -2032,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54">
@@ -2053,7 +2053,7 @@
         <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>0</v>
@@ -2062,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="H54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
@@ -2089,10 +2089,10 @@
         <v>1</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
@@ -2116,13 +2116,13 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" t="n">
         <v>1</v>
       </c>
       <c r="H56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
@@ -2152,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -2173,7 +2173,7 @@
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
@@ -2182,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="H58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -2206,13 +2206,13 @@
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" t="n">
         <v>0</v>
       </c>
       <c r="H59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -2239,10 +2239,10 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -2263,7 +2263,7 @@
         <v>1</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>1</v>
@@ -2272,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="H61" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62">
@@ -2290,7 +2290,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" t="n">
         <v>1</v>
@@ -2302,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="H62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -2326,13 +2326,13 @@
         <v>1</v>
       </c>
       <c r="F63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G63" t="n">
         <v>0</v>
       </c>
       <c r="H63" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64">
@@ -2359,10 +2359,10 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -2380,7 +2380,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -2392,7 +2392,7 @@
         <v>1</v>
       </c>
       <c r="H65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
@@ -2413,7 +2413,7 @@
         <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
@@ -2422,7 +2422,7 @@
         <v>0</v>
       </c>
       <c r="H66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -2446,13 +2446,13 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G67" t="n">
         <v>0</v>
       </c>
       <c r="H67" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
@@ -2479,10 +2479,10 @@
         <v>1</v>
       </c>
       <c r="G68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H68" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69">
@@ -2506,13 +2506,13 @@
         <v>1</v>
       </c>
       <c r="F69" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G69" t="n">
         <v>0</v>
       </c>
       <c r="H69" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
@@ -2533,7 +2533,7 @@
         <v>1</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
@@ -2542,7 +2542,7 @@
         <v>0</v>
       </c>
       <c r="H70" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -2560,7 +2560,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="n">
         <v>2</v>
@@ -2572,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72">
@@ -2599,10 +2599,10 @@
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -2623,7 +2623,7 @@
         <v>2</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
@@ -2632,7 +2632,7 @@
         <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74">
@@ -2650,7 +2650,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E74" t="n">
         <v>2</v>
@@ -2662,7 +2662,7 @@
         <v>0</v>
       </c>
       <c r="H74" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75">
@@ -2689,10 +2689,10 @@
         <v>2</v>
       </c>
       <c r="G75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H75" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76">
@@ -2716,13 +2716,13 @@
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G76" t="n">
         <v>2</v>
       </c>
       <c r="H76" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77">
@@ -2740,7 +2740,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
@@ -2752,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="H77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -2773,7 +2773,7 @@
         <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
@@ -2782,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="H78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -2806,13 +2806,13 @@
         <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79" t="n">
         <v>0</v>
       </c>
       <c r="H79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -2839,10 +2839,10 @@
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -2860,7 +2860,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
@@ -2872,7 +2872,7 @@
         <v>0</v>
       </c>
       <c r="H81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -2893,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>0</v>
@@ -2902,7 +2902,7 @@
         <v>0</v>
       </c>
       <c r="H82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -2926,13 +2926,13 @@
         <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G83" t="n">
         <v>1</v>
       </c>
       <c r="H83" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84">
@@ -2959,10 +2959,10 @@
         <v>1</v>
       </c>
       <c r="G84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H84" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85">
@@ -2983,7 +2983,7 @@
         <v>2</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -2992,7 +2992,7 @@
         <v>0</v>
       </c>
       <c r="H85" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86">
@@ -3010,7 +3010,7 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E86" t="n">
         <v>2</v>
@@ -3022,7 +3022,7 @@
         <v>0</v>
       </c>
       <c r="H86" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87">
@@ -3046,13 +3046,13 @@
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G87" t="n">
         <v>0</v>
       </c>
       <c r="H87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -3070,7 +3070,7 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E88" t="n">
         <v>0</v>
@@ -3082,7 +3082,7 @@
         <v>0</v>
       </c>
       <c r="H88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3103,7 +3103,7 @@
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>1</v>
@@ -3112,7 +3112,7 @@
         <v>0</v>
       </c>
       <c r="H89" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90">
@@ -3136,13 +3136,13 @@
         <v>1</v>
       </c>
       <c r="F90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G90" t="n">
         <v>0</v>
       </c>
       <c r="H90" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91">
@@ -3169,10 +3169,10 @@
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -3190,7 +3190,7 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" t="n">
         <v>0</v>
@@ -3202,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="H92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -3223,7 +3223,7 @@
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>0</v>
@@ -3232,7 +3232,7 @@
         <v>0</v>
       </c>
       <c r="H93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -3256,13 +3256,13 @@
         <v>0</v>
       </c>
       <c r="F94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G94" t="n">
         <v>0</v>
       </c>
       <c r="H94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -3289,10 +3289,10 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -3310,7 +3310,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E96" t="n">
         <v>1</v>
@@ -3322,7 +3322,7 @@
         <v>0</v>
       </c>
       <c r="H96" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97">
@@ -3343,7 +3343,7 @@
         <v>1</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>0</v>
@@ -3352,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="H97" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98">
@@ -3376,13 +3376,13 @@
         <v>0</v>
       </c>
       <c r="F98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98" t="n">
         <v>0</v>
       </c>
       <c r="H98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -3409,10 +3409,10 @@
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -3430,7 +3430,7 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
@@ -3442,7 +3442,7 @@
         <v>0</v>
       </c>
       <c r="H100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -3463,7 +3463,7 @@
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" t="n">
         <v>0</v>
@@ -3472,7 +3472,7 @@
         <v>0</v>
       </c>
       <c r="H101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -3499,10 +3499,10 @@
         <v>1</v>
       </c>
       <c r="G102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103">
@@ -3526,13 +3526,13 @@
         <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G103" t="n">
         <v>1</v>
       </c>
       <c r="H103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
@@ -3550,7 +3550,7 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E104" t="n">
         <v>2</v>
@@ -3562,7 +3562,7 @@
         <v>0</v>
       </c>
       <c r="H104" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105">
@@ -3583,7 +3583,7 @@
         <v>2</v>
       </c>
       <c r="E105" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F105" t="n">
         <v>0</v>
@@ -3592,7 +3592,7 @@
         <v>0</v>
       </c>
       <c r="H105" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106">
@@ -3616,13 +3616,13 @@
         <v>0</v>
       </c>
       <c r="F106" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G106" t="n">
         <v>2</v>
       </c>
       <c r="H106" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107">
@@ -3649,10 +3649,10 @@
         <v>2</v>
       </c>
       <c r="G107" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H107" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108">
@@ -3670,7 +3670,7 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E108" t="n">
         <v>0</v>
@@ -3682,7 +3682,7 @@
         <v>0</v>
       </c>
       <c r="H108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -3703,7 +3703,7 @@
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F109" t="n">
         <v>0</v>
@@ -3712,7 +3712,7 @@
         <v>0</v>
       </c>
       <c r="H109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -3736,13 +3736,13 @@
         <v>0</v>
       </c>
       <c r="F110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G110" t="n">
         <v>1</v>
       </c>
       <c r="H110" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111">
@@ -3769,10 +3769,10 @@
         <v>1</v>
       </c>
       <c r="G111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H111" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112">
@@ -3790,7 +3790,7 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112" t="n">
         <v>0</v>
@@ -3802,7 +3802,7 @@
         <v>0</v>
       </c>
       <c r="H112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
@@ -3826,13 +3826,13 @@
         <v>2</v>
       </c>
       <c r="F113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G113" t="n">
         <v>0</v>
       </c>
       <c r="H113" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114">
@@ -3853,7 +3853,7 @@
         <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F114" t="n">
         <v>2</v>
@@ -3862,7 +3862,7 @@
         <v>0</v>
       </c>
       <c r="H114" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
@@ -3889,10 +3889,10 @@
         <v>0</v>
       </c>
       <c r="G115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -3910,7 +3910,7 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E116" t="n">
         <v>0</v>
@@ -3922,7 +3922,7 @@
         <v>0</v>
       </c>
       <c r="H116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -3943,7 +3943,7 @@
         <v>0</v>
       </c>
       <c r="E117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F117" t="n">
         <v>1</v>
@@ -3952,7 +3952,7 @@
         <v>0</v>
       </c>
       <c r="H117" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118">
@@ -3976,13 +3976,13 @@
         <v>1</v>
       </c>
       <c r="F118" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G118" t="n">
         <v>0</v>
       </c>
       <c r="H118" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119">
@@ -4009,10 +4009,10 @@
         <v>0</v>
       </c>
       <c r="G119" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H119" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120">
@@ -4030,7 +4030,7 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E120" t="n">
         <v>0</v>
@@ -4042,7 +4042,7 @@
         <v>0</v>
       </c>
       <c r="H120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -4066,13 +4066,13 @@
         <v>1</v>
       </c>
       <c r="F121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G121" t="n">
         <v>0</v>
       </c>
       <c r="H121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122">
@@ -4093,7 +4093,7 @@
         <v>0</v>
       </c>
       <c r="E122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F122" t="n">
         <v>1</v>
@@ -4102,7 +4102,7 @@
         <v>0</v>
       </c>
       <c r="H122" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123">
@@ -4129,10 +4129,10 @@
         <v>0</v>
       </c>
       <c r="G123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124">
@@ -4150,7 +4150,7 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124" t="n">
         <v>0</v>
@@ -4162,7 +4162,7 @@
         <v>0</v>
       </c>
       <c r="H124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
@@ -4183,7 +4183,7 @@
         <v>0</v>
       </c>
       <c r="E125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F125" t="n">
         <v>0</v>
@@ -4192,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="H125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
@@ -4216,13 +4216,13 @@
         <v>0</v>
       </c>
       <c r="F126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G126" t="n">
         <v>0</v>
       </c>
       <c r="H126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
@@ -4249,10 +4249,10 @@
         <v>0</v>
       </c>
       <c r="G127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128">
@@ -4270,7 +4270,7 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E128" t="n">
         <v>0</v>
@@ -4282,7 +4282,7 @@
         <v>0</v>
       </c>
       <c r="H128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -4303,7 +4303,7 @@
         <v>0</v>
       </c>
       <c r="E129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F129" t="n">
         <v>1</v>
@@ -4312,7 +4312,7 @@
         <v>0</v>
       </c>
       <c r="H129" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130">
@@ -4336,13 +4336,13 @@
         <v>1</v>
       </c>
       <c r="F130" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G130" t="n">
         <v>0</v>
       </c>
       <c r="H130" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131">
@@ -4369,10 +4369,10 @@
         <v>0</v>
       </c>
       <c r="G131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132">
@@ -4390,7 +4390,7 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E132" t="n">
         <v>1</v>
@@ -4402,7 +4402,7 @@
         <v>0</v>
       </c>
       <c r="H132" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133">
@@ -4426,13 +4426,13 @@
         <v>2</v>
       </c>
       <c r="F133" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G133" t="n">
         <v>0</v>
       </c>
       <c r="H133" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134">
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
       <c r="E134" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F134" t="n">
         <v>2</v>
@@ -4462,7 +4462,7 @@
         <v>0</v>
       </c>
       <c r="H134" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135">
@@ -4489,10 +4489,10 @@
         <v>0</v>
       </c>
       <c r="G135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136">
@@ -4513,7 +4513,7 @@
         <v>1</v>
       </c>
       <c r="E136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F136" t="n">
         <v>0</v>
@@ -4522,7 +4522,7 @@
         <v>0</v>
       </c>
       <c r="H136" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
@@ -4540,7 +4540,7 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E137" t="n">
         <v>1</v>
@@ -4552,7 +4552,7 @@
         <v>0</v>
       </c>
       <c r="H137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138">
@@ -4576,13 +4576,13 @@
         <v>0</v>
       </c>
       <c r="F138" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G138" t="n">
         <v>1</v>
       </c>
       <c r="H138" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139">
@@ -4609,10 +4609,10 @@
         <v>1</v>
       </c>
       <c r="G139" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H139" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140">
@@ -4630,7 +4630,7 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E140" t="n">
         <v>0</v>
@@ -4642,7 +4642,7 @@
         <v>0</v>
       </c>
       <c r="H140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
@@ -4663,7 +4663,7 @@
         <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F141" t="n">
         <v>1</v>
@@ -4672,7 +4672,7 @@
         <v>0</v>
       </c>
       <c r="H141" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142">
@@ -4696,13 +4696,13 @@
         <v>1</v>
       </c>
       <c r="F142" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G142" t="n">
         <v>0</v>
       </c>
       <c r="H142" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143">
@@ -4729,10 +4729,10 @@
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -4750,7 +4750,7 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E144" t="n">
         <v>0</v>
@@ -4762,7 +4762,7 @@
         <v>0</v>
       </c>
       <c r="H144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
@@ -4783,7 +4783,7 @@
         <v>0</v>
       </c>
       <c r="E145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F145" t="n">
         <v>0</v>
@@ -4792,7 +4792,7 @@
         <v>0</v>
       </c>
       <c r="H145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146">
@@ -4816,13 +4816,13 @@
         <v>0</v>
       </c>
       <c r="F146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G146" t="n">
         <v>1</v>
       </c>
       <c r="H146" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147">
@@ -4849,10 +4849,10 @@
         <v>1</v>
       </c>
       <c r="G147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H147" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148">
@@ -4870,7 +4870,7 @@
         </is>
       </c>
       <c r="D148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E148" t="n">
         <v>0</v>
@@ -4882,7 +4882,7 @@
         <v>0</v>
       </c>
       <c r="H148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -4903,7 +4903,7 @@
         <v>0</v>
       </c>
       <c r="E149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F149" t="n">
         <v>0</v>
@@ -4912,7 +4912,7 @@
         <v>0</v>
       </c>
       <c r="H149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
@@ -4936,13 +4936,13 @@
         <v>0</v>
       </c>
       <c r="F150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G150" t="n">
         <v>0</v>
       </c>
       <c r="H150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
@@ -4969,10 +4969,10 @@
         <v>0</v>
       </c>
       <c r="G151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">
@@ -4990,7 +4990,7 @@
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E152" t="n">
         <v>0</v>
@@ -5002,7 +5002,7 @@
         <v>0</v>
       </c>
       <c r="H152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
@@ -5026,13 +5026,13 @@
         <v>1</v>
       </c>
       <c r="F153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G153" t="n">
         <v>0</v>
       </c>
       <c r="H153" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154">
@@ -5053,7 +5053,7 @@
         <v>0</v>
       </c>
       <c r="E154" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F154" t="n">
         <v>1</v>
@@ -5062,7 +5062,7 @@
         <v>0</v>
       </c>
       <c r="H154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155">
@@ -5089,10 +5089,10 @@
         <v>0</v>
       </c>
       <c r="G155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
@@ -5110,7 +5110,7 @@
         </is>
       </c>
       <c r="D156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E156" t="n">
         <v>0</v>
@@ -5122,7 +5122,7 @@
         <v>0</v>
       </c>
       <c r="H156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -5143,7 +5143,7 @@
         <v>0</v>
       </c>
       <c r="E157" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F157" t="n">
         <v>2</v>
@@ -5152,7 +5152,7 @@
         <v>1</v>
       </c>
       <c r="H157" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158">
@@ -5176,13 +5176,13 @@
         <v>2</v>
       </c>
       <c r="F158" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G158" t="n">
         <v>1</v>
       </c>
       <c r="H158" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="159">
@@ -5209,10 +5209,10 @@
         <v>1</v>
       </c>
       <c r="G159" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H159" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="160">
@@ -5230,7 +5230,7 @@
         </is>
       </c>
       <c r="D160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E160" t="n">
         <v>0</v>
@@ -5242,7 +5242,7 @@
         <v>0</v>
       </c>
       <c r="H160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -5266,13 +5266,13 @@
         <v>1</v>
       </c>
       <c r="F161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G161" t="n">
         <v>0</v>
       </c>
       <c r="H161" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162">
@@ -5293,7 +5293,7 @@
         <v>0</v>
       </c>
       <c r="E162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F162" t="n">
         <v>1</v>
@@ -5302,7 +5302,7 @@
         <v>0</v>
       </c>
       <c r="H162" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163">
@@ -5329,10 +5329,10 @@
         <v>0</v>
       </c>
       <c r="G163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -5350,7 +5350,7 @@
         </is>
       </c>
       <c r="D164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E164" t="n">
         <v>0</v>
@@ -5362,7 +5362,7 @@
         <v>0</v>
       </c>
       <c r="H164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -5383,7 +5383,7 @@
         <v>0</v>
       </c>
       <c r="E165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F165" t="n">
         <v>0</v>
@@ -5392,7 +5392,7 @@
         <v>0</v>
       </c>
       <c r="H165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166">
@@ -5416,13 +5416,13 @@
         <v>0</v>
       </c>
       <c r="F166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G166" t="n">
         <v>0</v>
       </c>
       <c r="H166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167">
@@ -5449,10 +5449,10 @@
         <v>0</v>
       </c>
       <c r="G167" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H167" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -5470,7 +5470,7 @@
         </is>
       </c>
       <c r="D168" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E168" t="n">
         <v>0</v>
@@ -5482,7 +5482,7 @@
         <v>0</v>
       </c>
       <c r="H168" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -5503,7 +5503,7 @@
         <v>0</v>
       </c>
       <c r="E169" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F169" t="n">
         <v>0</v>
@@ -5512,7 +5512,7 @@
         <v>0</v>
       </c>
       <c r="H169" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -5539,10 +5539,10 @@
         <v>1</v>
       </c>
       <c r="G170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171">
@@ -5566,13 +5566,13 @@
         <v>0</v>
       </c>
       <c r="F171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G171" t="n">
         <v>1</v>
       </c>
       <c r="H171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172">
@@ -5590,7 +5590,7 @@
         </is>
       </c>
       <c r="D172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E172" t="n">
         <v>0</v>
@@ -5602,7 +5602,7 @@
         <v>0</v>
       </c>
       <c r="H172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -5623,7 +5623,7 @@
         <v>0</v>
       </c>
       <c r="E173" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F173" t="n">
         <v>1</v>
@@ -5632,7 +5632,7 @@
         <v>0</v>
       </c>
       <c r="H173" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174">
@@ -5656,13 +5656,13 @@
         <v>1</v>
       </c>
       <c r="F174" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G174" t="n">
         <v>0</v>
       </c>
       <c r="H174" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="175">
@@ -5689,10 +5689,10 @@
         <v>0</v>
       </c>
       <c r="G175" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H175" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176">
@@ -5713,7 +5713,7 @@
         <v>1</v>
       </c>
       <c r="E176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F176" t="n">
         <v>1</v>
@@ -5722,7 +5722,7 @@
         <v>0</v>
       </c>
       <c r="H176" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177">
@@ -5746,13 +5746,13 @@
         <v>1</v>
       </c>
       <c r="F177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G177" t="n">
         <v>0</v>
       </c>
       <c r="H177" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178">
@@ -5770,7 +5770,7 @@
         </is>
       </c>
       <c r="D178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E178" t="n">
         <v>1</v>
@@ -5782,7 +5782,7 @@
         <v>0</v>
       </c>
       <c r="H178" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179">
@@ -5809,10 +5809,10 @@
         <v>0</v>
       </c>
       <c r="G179" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H179" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180">
@@ -5833,7 +5833,7 @@
         <v>1</v>
       </c>
       <c r="E180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F180" t="n">
         <v>0</v>
@@ -5842,7 +5842,7 @@
         <v>0</v>
       </c>
       <c r="H180" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181">
@@ -5860,7 +5860,7 @@
         </is>
       </c>
       <c r="D181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E181" t="n">
         <v>1</v>
@@ -5872,7 +5872,7 @@
         <v>0</v>
       </c>
       <c r="H181" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182">
@@ -5899,10 +5899,10 @@
         <v>1</v>
       </c>
       <c r="G182" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H182" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183">
@@ -5926,13 +5926,13 @@
         <v>0</v>
       </c>
       <c r="F183" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G183" t="n">
         <v>1</v>
       </c>
       <c r="H183" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184">
@@ -5950,7 +5950,7 @@
         </is>
       </c>
       <c r="D184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E184" t="n">
         <v>0</v>
@@ -5962,7 +5962,7 @@
         <v>0</v>
       </c>
       <c r="H184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
@@ -5986,13 +5986,13 @@
         <v>1</v>
       </c>
       <c r="F185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G185" t="n">
         <v>0</v>
       </c>
       <c r="H185" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186">
@@ -6013,7 +6013,7 @@
         <v>0</v>
       </c>
       <c r="E186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F186" t="n">
         <v>1</v>
@@ -6022,7 +6022,7 @@
         <v>0</v>
       </c>
       <c r="H186" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187">
@@ -6049,10 +6049,10 @@
         <v>0</v>
       </c>
       <c r="G187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188">
@@ -6070,7 +6070,7 @@
         </is>
       </c>
       <c r="D188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E188" t="n">
         <v>0</v>
@@ -6082,7 +6082,7 @@
         <v>0</v>
       </c>
       <c r="H188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">
@@ -6109,10 +6109,10 @@
         <v>0</v>
       </c>
       <c r="G189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H189" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190">
@@ -6136,13 +6136,13 @@
         <v>0</v>
       </c>
       <c r="F190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G190" t="n">
         <v>0</v>
       </c>
       <c r="H190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191">
@@ -6163,7 +6163,7 @@
         <v>0</v>
       </c>
       <c r="E191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F191" t="n">
         <v>0</v>
@@ -6172,7 +6172,7 @@
         <v>1</v>
       </c>
       <c r="H191" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="192">
@@ -6190,7 +6190,7 @@
         </is>
       </c>
       <c r="D192" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E192" t="n">
         <v>0</v>
@@ -6202,7 +6202,7 @@
         <v>0</v>
       </c>
       <c r="H192" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193">
@@ -6223,7 +6223,7 @@
         <v>0</v>
       </c>
       <c r="E193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F193" t="n">
         <v>0</v>
@@ -6232,7 +6232,7 @@
         <v>0</v>
       </c>
       <c r="H193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
@@ -6256,13 +6256,13 @@
         <v>0</v>
       </c>
       <c r="F194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G194" t="n">
         <v>0</v>
       </c>
       <c r="H194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195">
@@ -6289,10 +6289,10 @@
         <v>0</v>
       </c>
       <c r="G195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
@@ -6313,7 +6313,7 @@
         <v>1</v>
       </c>
       <c r="E196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F196" t="n">
         <v>0</v>
@@ -6322,7 +6322,7 @@
         <v>0</v>
       </c>
       <c r="H196" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="197">
@@ -6340,7 +6340,7 @@
         </is>
       </c>
       <c r="D197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E197" t="n">
         <v>1</v>
@@ -6352,7 +6352,7 @@
         <v>0</v>
       </c>
       <c r="H197" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="198">
@@ -6376,13 +6376,13 @@
         <v>0</v>
       </c>
       <c r="F198" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G198" t="n">
         <v>0</v>
       </c>
       <c r="H198" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="199">
@@ -6409,10 +6409,10 @@
         <v>0</v>
       </c>
       <c r="G199" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H199" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="200">
@@ -6430,7 +6430,7 @@
         </is>
       </c>
       <c r="D200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E200" t="n">
         <v>0</v>
@@ -6442,7 +6442,7 @@
         <v>0</v>
       </c>
       <c r="H200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201">
@@ -6463,7 +6463,7 @@
         <v>0</v>
       </c>
       <c r="E201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F201" t="n">
         <v>0</v>
@@ -6472,7 +6472,7 @@
         <v>0</v>
       </c>
       <c r="H201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202">
@@ -6496,13 +6496,13 @@
         <v>0</v>
       </c>
       <c r="F202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G202" t="n">
         <v>0</v>
       </c>
       <c r="H202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203">
@@ -6529,10 +6529,10 @@
         <v>0</v>
       </c>
       <c r="G203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204">
@@ -6550,7 +6550,7 @@
         </is>
       </c>
       <c r="D204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E204" t="n">
         <v>0</v>
@@ -6562,7 +6562,7 @@
         <v>0</v>
       </c>
       <c r="H204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205">
@@ -6583,7 +6583,7 @@
         <v>0</v>
       </c>
       <c r="E205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F205" t="n">
         <v>0</v>
@@ -6592,7 +6592,7 @@
         <v>0</v>
       </c>
       <c r="H205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206">
@@ -6619,10 +6619,10 @@
         <v>1</v>
       </c>
       <c r="G206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H206" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="207">
@@ -6646,13 +6646,13 @@
         <v>0</v>
       </c>
       <c r="F207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G207" t="n">
         <v>1</v>
       </c>
       <c r="H207" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="208">
@@ -6670,7 +6670,7 @@
         </is>
       </c>
       <c r="D208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E208" t="n">
         <v>0</v>
@@ -6682,7 +6682,7 @@
         <v>0</v>
       </c>
       <c r="H208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209">
@@ -6709,10 +6709,10 @@
         <v>2</v>
       </c>
       <c r="G209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H209" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="210">
@@ -6733,7 +6733,7 @@
         <v>0</v>
       </c>
       <c r="E210" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F210" t="n">
         <v>2</v>
@@ -6742,7 +6742,7 @@
         <v>0</v>
       </c>
       <c r="H210" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="211">
@@ -6766,13 +6766,13 @@
         <v>0</v>
       </c>
       <c r="F211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G211" t="n">
         <v>1</v>
       </c>
       <c r="H211" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="212">
@@ -6790,7 +6790,7 @@
         </is>
       </c>
       <c r="D212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E212" t="n">
         <v>0</v>
@@ -6802,7 +6802,7 @@
         <v>0</v>
       </c>
       <c r="H212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213">
@@ -6826,13 +6826,13 @@
         <v>1</v>
       </c>
       <c r="F213" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G213" t="n">
         <v>0</v>
       </c>
       <c r="H213" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214">
@@ -6853,7 +6853,7 @@
         <v>0</v>
       </c>
       <c r="E214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F214" t="n">
         <v>1</v>
@@ -6862,7 +6862,7 @@
         <v>0</v>
       </c>
       <c r="H214" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="215">
@@ -6889,10 +6889,10 @@
         <v>0</v>
       </c>
       <c r="G215" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H215" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="216">
@@ -6910,7 +6910,7 @@
         </is>
       </c>
       <c r="D216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E216" t="n">
         <v>0</v>
@@ -6922,7 +6922,7 @@
         <v>0</v>
       </c>
       <c r="H216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">
@@ -6946,13 +6946,13 @@
         <v>1</v>
       </c>
       <c r="F217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G217" t="n">
         <v>0</v>
       </c>
       <c r="H217" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="218">
@@ -6973,7 +6973,7 @@
         <v>0</v>
       </c>
       <c r="E218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F218" t="n">
         <v>1</v>
@@ -6982,7 +6982,7 @@
         <v>0</v>
       </c>
       <c r="H218" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="219">
@@ -7009,10 +7009,10 @@
         <v>0</v>
       </c>
       <c r="G219" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H219" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220">
@@ -7030,7 +7030,7 @@
         </is>
       </c>
       <c r="D220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E220" t="n">
         <v>0</v>
@@ -7042,7 +7042,7 @@
         <v>0</v>
       </c>
       <c r="H220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221">
@@ -7066,13 +7066,13 @@
         <v>2</v>
       </c>
       <c r="F221" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G221" t="n">
         <v>0</v>
       </c>
       <c r="H221" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="222">
@@ -7093,7 +7093,7 @@
         <v>0</v>
       </c>
       <c r="E222" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F222" t="n">
         <v>2</v>
@@ -7102,7 +7102,7 @@
         <v>0</v>
       </c>
       <c r="H222" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="223">
@@ -7129,10 +7129,10 @@
         <v>0</v>
       </c>
       <c r="G223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224">
@@ -7150,7 +7150,7 @@
         </is>
       </c>
       <c r="D224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E224" t="n">
         <v>0</v>
@@ -7162,7 +7162,7 @@
         <v>0</v>
       </c>
       <c r="H224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225">
@@ -7183,7 +7183,7 @@
         <v>0</v>
       </c>
       <c r="E225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F225" t="n">
         <v>0</v>
@@ -7192,7 +7192,7 @@
         <v>0</v>
       </c>
       <c r="H225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226">
@@ -7219,10 +7219,10 @@
         <v>2</v>
       </c>
       <c r="G226" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H226" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="227">
@@ -7246,13 +7246,13 @@
         <v>0</v>
       </c>
       <c r="F227" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G227" t="n">
         <v>2</v>
       </c>
       <c r="H227" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="228">
@@ -7270,7 +7270,7 @@
         </is>
       </c>
       <c r="D228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E228" t="n">
         <v>0</v>
@@ -7282,7 +7282,7 @@
         <v>0</v>
       </c>
       <c r="H228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229">
@@ -7303,7 +7303,7 @@
         <v>0</v>
       </c>
       <c r="E229" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F229" t="n">
         <v>1</v>
@@ -7312,7 +7312,7 @@
         <v>0</v>
       </c>
       <c r="H229" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="230">
@@ -7336,13 +7336,13 @@
         <v>1</v>
       </c>
       <c r="F230" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G230" t="n">
         <v>0</v>
       </c>
       <c r="H230" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="231">
@@ -7369,10 +7369,10 @@
         <v>0</v>
       </c>
       <c r="G231" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H231" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="232">
@@ -7393,7 +7393,7 @@
         <v>1</v>
       </c>
       <c r="E232" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F232" t="n">
         <v>0</v>
@@ -7402,7 +7402,7 @@
         <v>0</v>
       </c>
       <c r="H232" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="233">
@@ -7420,7 +7420,7 @@
         </is>
       </c>
       <c r="D233" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E233" t="n">
         <v>1</v>
@@ -7432,7 +7432,7 @@
         <v>0</v>
       </c>
       <c r="H233" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="234">
@@ -7459,10 +7459,10 @@
         <v>1</v>
       </c>
       <c r="G234" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H234" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="235">
@@ -7486,13 +7486,13 @@
         <v>0</v>
       </c>
       <c r="F235" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G235" t="n">
         <v>1</v>
       </c>
       <c r="H235" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236">
@@ -7513,7 +7513,7 @@
         <v>2</v>
       </c>
       <c r="E236" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F236" t="n">
         <v>0</v>
@@ -7522,7 +7522,7 @@
         <v>0</v>
       </c>
       <c r="H236" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="237">
@@ -7540,7 +7540,7 @@
         </is>
       </c>
       <c r="D237" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E237" t="n">
         <v>2</v>
@@ -7552,7 +7552,7 @@
         <v>0</v>
       </c>
       <c r="H237" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="238">
@@ -7579,10 +7579,10 @@
         <v>1</v>
       </c>
       <c r="G238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H238" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="239">
@@ -7606,13 +7606,13 @@
         <v>0</v>
       </c>
       <c r="F239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G239" t="n">
         <v>1</v>
       </c>
       <c r="H239" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="240">
@@ -7633,7 +7633,7 @@
         <v>1</v>
       </c>
       <c r="E240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F240" t="n">
         <v>0</v>
@@ -7642,7 +7642,7 @@
         <v>0</v>
       </c>
       <c r="H240" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="241">
@@ -7660,7 +7660,7 @@
         </is>
       </c>
       <c r="D241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E241" t="n">
         <v>1</v>
@@ -7672,7 +7672,7 @@
         <v>0</v>
       </c>
       <c r="H241" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="242">
@@ -7699,10 +7699,10 @@
         <v>1</v>
       </c>
       <c r="G242" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H242" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="243">
@@ -7726,13 +7726,13 @@
         <v>0</v>
       </c>
       <c r="F243" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G243" t="n">
         <v>1</v>
       </c>
       <c r="H243" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="244">
@@ -7750,7 +7750,7 @@
         </is>
       </c>
       <c r="D244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E244" t="n">
         <v>0</v>
@@ -7762,7 +7762,7 @@
         <v>0</v>
       </c>
       <c r="H244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245">
@@ -7789,10 +7789,10 @@
         <v>1</v>
       </c>
       <c r="G245" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H245" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="246">
@@ -7813,7 +7813,7 @@
         <v>0</v>
       </c>
       <c r="E246" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F246" t="n">
         <v>2</v>
@@ -7822,7 +7822,7 @@
         <v>0</v>
       </c>
       <c r="H246" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="247">
@@ -7846,13 +7846,13 @@
         <v>0</v>
       </c>
       <c r="F247" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G247" t="n">
         <v>3</v>
       </c>
       <c r="H247" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="248">
@@ -7870,7 +7870,7 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E248" t="n">
         <v>1</v>
@@ -7882,7 +7882,7 @@
         <v>0</v>
       </c>
       <c r="H248" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="249">
@@ -7903,7 +7903,7 @@
         <v>1</v>
       </c>
       <c r="E249" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F249" t="n">
         <v>0</v>
@@ -7912,7 +7912,7 @@
         <v>0</v>
       </c>
       <c r="H249" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="250">
@@ -7936,13 +7936,13 @@
         <v>0</v>
       </c>
       <c r="F250" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G250" t="n">
         <v>0</v>
       </c>
       <c r="H250" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="251">
@@ -7969,10 +7969,10 @@
         <v>0</v>
       </c>
       <c r="G251" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H251" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="252">
@@ -7996,13 +7996,13 @@
         <v>1</v>
       </c>
       <c r="F252" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G252" t="n">
         <v>0</v>
       </c>
       <c r="H252" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="253">
@@ -8020,7 +8020,7 @@
         </is>
       </c>
       <c r="D253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E253" t="n">
         <v>1</v>
@@ -8032,7 +8032,7 @@
         <v>0</v>
       </c>
       <c r="H253" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="254">
@@ -8059,10 +8059,10 @@
         <v>1</v>
       </c>
       <c r="G254" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H254" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="255">
@@ -8083,7 +8083,7 @@
         <v>0</v>
       </c>
       <c r="E255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F255" t="n">
         <v>1</v>
@@ -8092,7 +8092,7 @@
         <v>1</v>
       </c>
       <c r="H255" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="256">
@@ -8110,7 +8110,7 @@
         </is>
       </c>
       <c r="D256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E256" t="n">
         <v>0</v>
@@ -8122,7 +8122,7 @@
         <v>0</v>
       </c>
       <c r="H256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257">
@@ -8143,7 +8143,7 @@
         <v>0</v>
       </c>
       <c r="E257" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F257" t="n">
         <v>0</v>
@@ -8152,7 +8152,7 @@
         <v>0</v>
       </c>
       <c r="H257" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="258">
@@ -8176,13 +8176,13 @@
         <v>0</v>
       </c>
       <c r="F258" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G258" t="n">
         <v>1</v>
       </c>
       <c r="H258" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="259">
@@ -8209,10 +8209,10 @@
         <v>1</v>
       </c>
       <c r="G259" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H259" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="260">
@@ -8233,7 +8233,7 @@
         <v>1</v>
       </c>
       <c r="E260" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F260" t="n">
         <v>0</v>
@@ -8242,7 +8242,7 @@
         <v>0</v>
       </c>
       <c r="H260" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="261">
@@ -8260,7 +8260,7 @@
         </is>
       </c>
       <c r="D261" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E261" t="n">
         <v>1</v>
@@ -8272,7 +8272,7 @@
         <v>0</v>
       </c>
       <c r="H261" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="262">
@@ -8299,10 +8299,10 @@
         <v>1</v>
       </c>
       <c r="G262" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H262" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263">
@@ -8326,13 +8326,13 @@
         <v>0</v>
       </c>
       <c r="F263" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G263" t="n">
         <v>1</v>
       </c>
       <c r="H263" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264">
@@ -8470,7 +8470,7 @@
         </is>
       </c>
       <c r="D268" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E268" t="n">
         <v>0</v>
@@ -8482,7 +8482,7 @@
         <v>0</v>
       </c>
       <c r="H268" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269">
@@ -8506,13 +8506,13 @@
         <v>1</v>
       </c>
       <c r="F269" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G269" t="n">
         <v>0</v>
       </c>
       <c r="H269" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="270">
@@ -8533,7 +8533,7 @@
         <v>0</v>
       </c>
       <c r="E270" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F270" t="n">
         <v>1</v>
@@ -8542,7 +8542,7 @@
         <v>0</v>
       </c>
       <c r="H270" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="271">
@@ -8569,10 +8569,10 @@
         <v>0</v>
       </c>
       <c r="G271" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H271" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="272">
@@ -8593,7 +8593,7 @@
         <v>1</v>
       </c>
       <c r="E272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F272" t="n">
         <v>0</v>
@@ -8602,7 +8602,7 @@
         <v>0</v>
       </c>
       <c r="H272" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="273">
@@ -8620,7 +8620,7 @@
         </is>
       </c>
       <c r="D273" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E273" t="n">
         <v>1</v>
@@ -8632,7 +8632,7 @@
         <v>0</v>
       </c>
       <c r="H273" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="274">
@@ -8659,10 +8659,10 @@
         <v>1</v>
       </c>
       <c r="G274" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H274" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="275">
@@ -8686,13 +8686,13 @@
         <v>0</v>
       </c>
       <c r="F275" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G275" t="n">
         <v>1</v>
       </c>
       <c r="H275" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="276">
@@ -8710,7 +8710,7 @@
         </is>
       </c>
       <c r="D276" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E276" t="n">
         <v>0</v>
@@ -8722,7 +8722,7 @@
         <v>0</v>
       </c>
       <c r="H276" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="277">
@@ -8743,7 +8743,7 @@
         <v>0</v>
       </c>
       <c r="E277" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F277" t="n">
         <v>1</v>
@@ -8752,7 +8752,7 @@
         <v>0</v>
       </c>
       <c r="H277" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="278">
@@ -8779,10 +8779,10 @@
         <v>1</v>
       </c>
       <c r="G278" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H278" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="279">
@@ -8806,13 +8806,13 @@
         <v>0</v>
       </c>
       <c r="F279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G279" t="n">
         <v>1</v>
       </c>
       <c r="H279" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="280">
@@ -8833,7 +8833,7 @@
         <v>1</v>
       </c>
       <c r="E280" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F280" t="n">
         <v>1</v>
@@ -8842,7 +8842,7 @@
         <v>0</v>
       </c>
       <c r="H280" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="281">
@@ -8860,7 +8860,7 @@
         </is>
       </c>
       <c r="D281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E281" t="n">
         <v>2</v>
@@ -8872,7 +8872,7 @@
         <v>0</v>
       </c>
       <c r="H281" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="282">
@@ -8899,10 +8899,10 @@
         <v>2</v>
       </c>
       <c r="G282" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H282" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="283">
@@ -8926,13 +8926,13 @@
         <v>1</v>
       </c>
       <c r="F283" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G283" t="n">
         <v>2</v>
       </c>
       <c r="H283" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="284">
@@ -8953,7 +8953,7 @@
         <v>1</v>
       </c>
       <c r="E284" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F284" t="n">
         <v>0</v>
@@ -8962,7 +8962,7 @@
         <v>0</v>
       </c>
       <c r="H284" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="285">
@@ -8980,7 +8980,7 @@
         </is>
       </c>
       <c r="D285" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E285" t="n">
         <v>1</v>
@@ -8992,7 +8992,7 @@
         <v>0</v>
       </c>
       <c r="H285" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="286">
@@ -9016,13 +9016,13 @@
         <v>0</v>
       </c>
       <c r="F286" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G286" t="n">
         <v>0</v>
       </c>
       <c r="H286" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="287">
@@ -9049,10 +9049,10 @@
         <v>0</v>
       </c>
       <c r="G287" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H287" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="288">
@@ -9070,7 +9070,7 @@
         </is>
       </c>
       <c r="D288" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E288" t="n">
         <v>0</v>
@@ -9082,7 +9082,7 @@
         <v>0</v>
       </c>
       <c r="H288" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="289">
@@ -9103,7 +9103,7 @@
         <v>0</v>
       </c>
       <c r="E289" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F289" t="n">
         <v>1</v>
@@ -9112,7 +9112,7 @@
         <v>0</v>
       </c>
       <c r="H289" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="290">
@@ -9136,13 +9136,13 @@
         <v>0</v>
       </c>
       <c r="F290" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G290" t="n">
         <v>1</v>
       </c>
       <c r="H290" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="291">
@@ -9169,10 +9169,10 @@
         <v>0</v>
       </c>
       <c r="G291" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H291" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="292">
@@ -9190,7 +9190,7 @@
         </is>
       </c>
       <c r="D292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E292" t="n">
         <v>0</v>
@@ -9202,7 +9202,7 @@
         <v>0</v>
       </c>
       <c r="H292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293">
@@ -9226,13 +9226,13 @@
         <v>1</v>
       </c>
       <c r="F293" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G293" t="n">
         <v>1</v>
       </c>
       <c r="H293" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="294">
@@ -9259,10 +9259,10 @@
         <v>2</v>
       </c>
       <c r="G294" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H294" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="295">
@@ -9283,7 +9283,7 @@
         <v>0</v>
       </c>
       <c r="E295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F295" t="n">
         <v>1</v>
@@ -9292,7 +9292,7 @@
         <v>1</v>
       </c>
       <c r="H295" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>